<commit_message>
CISC 874 Project - Project Part C done ?
</commit_message>
<xml_diff>
--- a/CISC874/Project/PartC/CISC874-0bc15-ProjectPartC/NetworkPerformance.xlsx
+++ b/CISC874/Project/PartC/CISC874-0bc15-ProjectPartC/NetworkPerformance.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29070" windowHeight="15870"/>
   </bookViews>
   <sheets>
     <sheet name="Lavenberg-Marquardt" sheetId="1" r:id="rId1"/>
@@ -75,9 +75,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.000000"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -120,8 +121,8 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -140,7 +141,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -153,63 +154,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Average Curvature Error vs Noise StdDev</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -240,6 +185,103 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd" cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-9.9099882453343641E-2"/>
+                  <c:y val="0.32599479650196561"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                      <a:t>y = 0.1187x + 1.3911</a:t>
+                    </a:r>
+                    <a:br>
+                      <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                    </a:br>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                      <a:t>R² = 0.6127</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="1200"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>('Lavenberg-Marquardt'!$D$11,'Lavenberg-Marquardt'!$H$11,'Lavenberg-Marquardt'!$L$11,'Lavenberg-Marquardt'!$P$11,'Lavenberg-Marquardt'!$T$11,'Lavenberg-Marquardt'!$X$11,'Lavenberg-Marquardt'!$AB$11,'Lavenberg-Marquardt'!$AF$11,'Lavenberg-Marquardt'!$AJ$11,'Lavenberg-Marquardt'!$AN$11,'Lavenberg-Marquardt'!$AR$11)</c:f>
@@ -286,7 +328,7 @@
             <c:numRef>
               <c:f>('Lavenberg-Marquardt'!$E$73,'Lavenberg-Marquardt'!$I$73,'Lavenberg-Marquardt'!$M$73,'Lavenberg-Marquardt'!$Q$73,'Lavenberg-Marquardt'!$U$73,'Lavenberg-Marquardt'!$Y$73,'Lavenberg-Marquardt'!$AC$73,'Lavenberg-Marquardt'!$AG$73,'Lavenberg-Marquardt'!$AK$73,'Lavenberg-Marquardt'!$AO$73,'Lavenberg-Marquardt'!$AS$73)</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1.30328226</c:v>
@@ -325,7 +367,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-FE4B-4509-83CC-5EFBCF618029}"/>
             </c:ext>
@@ -339,11 +381,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="163149656"/>
-        <c:axId val="163147696"/>
+        <c:axId val="157867064"/>
+        <c:axId val="157863928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="163149656"/>
+        <c:axId val="157867064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -363,6 +405,71 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA" sz="1100"/>
+                  <a:t>Noise Standard Deviation (mm</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" sz="1100" baseline="30000"/>
+                  <a:t>2</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+                  <a:t>)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CA" sz="1100"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -400,12 +507,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="163147696"/>
+        <c:crossAx val="157863928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="163147696"/>
+        <c:axId val="157863928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -425,7 +532,76 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA" sz="1100"/>
+                  <a:t>Average Mean Squared</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+                  <a:t> Error (deg</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" sz="1100" baseline="30000"/>
+                  <a:t>2</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+                  <a:t>)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CA" sz="1100"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -462,7 +638,527 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="163149656"/>
+        <c:crossAx val="157867064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="9.4318869409433723E-3"/>
+                  <c:y val="0.1308172725120266"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                      <a:t>y = 0.0236x + 0.9513</a:t>
+                    </a:r>
+                    <a:br>
+                      <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                    </a:br>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                      <a:t>R² = 0.0762</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="1200"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Lavenberg-Marquardt'!$D$11,'Lavenberg-Marquardt'!$H$11,'Lavenberg-Marquardt'!$L$11,'Lavenberg-Marquardt'!$P$11,'Lavenberg-Marquardt'!$T$11,'Lavenberg-Marquardt'!$X$11,'Lavenberg-Marquardt'!$AB$11,'Lavenberg-Marquardt'!$AF$11,'Lavenberg-Marquardt'!$AJ$11,'Lavenberg-Marquardt'!$AN$11,'Lavenberg-Marquardt'!$AR$11)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Lavenberg-Marquardt'!$E$74,'Lavenberg-Marquardt'!$I$74,'Lavenberg-Marquardt'!$M$74,'Lavenberg-Marquardt'!$Q$74,'Lavenberg-Marquardt'!$U$74,'Lavenberg-Marquardt'!$Y$74,'Lavenberg-Marquardt'!$AC$74,'Lavenberg-Marquardt'!$AG$74,'Lavenberg-Marquardt'!$AK$74,'Lavenberg-Marquardt'!$AO$74,'Lavenberg-Marquardt'!$AS$74)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.0418522284963234</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.73538780367365142</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0416816642410021</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.72250033002512593</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2523707420669654</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6043563852196951</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1510664731392859</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.67427568198032706</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1326796183704566</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.3594251876732011</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0467784475970925</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="207713296"/>
+        <c:axId val="207712904"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="207713296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA" sz="1200"/>
+                  <a:t>Noise Standard Deviation (mm</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" sz="1200" baseline="30000"/>
+                  <a:t>2</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" sz="1200" baseline="0"/>
+                  <a:t>)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CA" sz="1200"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="207712904"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="207712904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA" sz="1200"/>
+                  <a:t>Standard</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" sz="1200" baseline="0"/>
+                  <a:t> Deviation of MSEs</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CA" sz="1200"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="207713296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -512,6 +1208,46 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1067,6 +1803,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1094,6 +2346,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>566737</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1367,8 +2649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AS74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R9" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+    <sheetView tabSelected="1" topLeftCell="Q17" workbookViewId="0">
+      <selection activeCell="V32" sqref="V32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2677,145 +3959,145 @@
       <c r="A42" t="s">
         <v>11</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C42" s="4">
         <f>AVERAGE(C16:C25)</f>
         <v>1.37523551E-3</v>
       </c>
-      <c r="D42" s="5">
+      <c r="D42" s="4">
         <f t="shared" ref="D42:I42" si="0">AVERAGE(D16:D25)</f>
         <v>6.8460190000000001E-3</v>
       </c>
-      <c r="E42" s="5">
+      <c r="E42" s="4">
         <f t="shared" si="0"/>
         <v>7.2404570000000005E-3</v>
       </c>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5">
+      <c r="F42" s="4"/>
+      <c r="G42" s="4">
         <f t="shared" si="0"/>
         <v>2.6092162288800002E-3</v>
       </c>
-      <c r="H42" s="5">
+      <c r="H42" s="4">
         <f t="shared" si="0"/>
         <v>6.6066569999999993E-3</v>
       </c>
-      <c r="I42" s="5">
+      <c r="I42" s="4">
         <f t="shared" si="0"/>
         <v>8.6891569999999994E-3</v>
       </c>
-      <c r="J42" s="5"/>
-      <c r="K42" s="5">
+      <c r="J42" s="4"/>
+      <c r="K42" s="4">
         <f t="shared" ref="K42:Y42" si="1">AVERAGE(K16:K25)</f>
         <v>1.0231905139153901E-3</v>
       </c>
-      <c r="L42" s="5">
+      <c r="L42" s="4">
         <f t="shared" si="1"/>
         <v>6.4684490000000011E-3</v>
       </c>
-      <c r="M42" s="5">
+      <c r="M42" s="4">
         <f t="shared" si="1"/>
         <v>7.2424059999999981E-3</v>
       </c>
-      <c r="N42" s="5"/>
-      <c r="O42" s="5">
+      <c r="N42" s="4"/>
+      <c r="O42" s="4">
         <f t="shared" si="1"/>
         <v>1.1321219820289957E-3</v>
       </c>
-      <c r="P42" s="5">
+      <c r="P42" s="4">
         <f t="shared" si="1"/>
         <v>6.8344909999999998E-3</v>
       </c>
-      <c r="Q42" s="5">
+      <c r="Q42" s="4">
         <f t="shared" si="1"/>
         <v>8.1493120000000006E-3</v>
       </c>
-      <c r="R42" s="5"/>
-      <c r="S42" s="5">
+      <c r="R42" s="4"/>
+      <c r="S42" s="4">
         <f t="shared" si="1"/>
         <v>3.3053918318800002E-3</v>
       </c>
-      <c r="T42" s="5">
+      <c r="T42" s="4">
         <f t="shared" si="1"/>
         <v>1.2876661000000001E-2</v>
       </c>
-      <c r="U42" s="5">
+      <c r="U42" s="4">
         <f t="shared" si="1"/>
         <v>1.398569E-2</v>
       </c>
-      <c r="V42" s="5"/>
-      <c r="W42" s="5">
+      <c r="V42" s="4"/>
+      <c r="W42" s="4">
         <f t="shared" si="1"/>
         <v>3.0978245417357998E-3</v>
       </c>
-      <c r="X42" s="5">
+      <c r="X42" s="4">
         <f t="shared" si="1"/>
         <v>7.9085519999999992E-3</v>
       </c>
-      <c r="Y42" s="5">
+      <c r="Y42" s="4">
         <f t="shared" si="1"/>
         <v>1.2411659E-2</v>
       </c>
-      <c r="Z42" s="5"/>
-      <c r="AA42" s="5">
-        <f t="shared" ref="Z42:AS42" si="2">AVERAGE(AA16:AA25)</f>
+      <c r="Z42" s="4"/>
+      <c r="AA42" s="4">
+        <f t="shared" ref="AA42:AS42" si="2">AVERAGE(AA16:AA25)</f>
         <v>1.5814564425502258E-3</v>
       </c>
-      <c r="AB42" s="5">
+      <c r="AB42" s="4">
         <f t="shared" si="2"/>
         <v>8.6757980000000002E-3</v>
       </c>
-      <c r="AC42" s="5">
+      <c r="AC42" s="4">
         <f t="shared" si="2"/>
         <v>1.3097407E-2</v>
       </c>
-      <c r="AD42" s="5"/>
-      <c r="AE42" s="5">
+      <c r="AD42" s="4"/>
+      <c r="AE42" s="4">
         <f t="shared" si="2"/>
         <v>2.3102208600000004E-3</v>
       </c>
-      <c r="AF42" s="5">
+      <c r="AF42" s="4">
         <f t="shared" si="2"/>
         <v>8.8849820000000013E-3</v>
       </c>
-      <c r="AG42" s="5">
+      <c r="AG42" s="4">
         <f t="shared" si="2"/>
         <v>1.0268302999999999E-2</v>
       </c>
-      <c r="AH42" s="5"/>
-      <c r="AI42" s="5">
+      <c r="AH42" s="4"/>
+      <c r="AI42" s="4">
         <f t="shared" si="2"/>
         <v>9.4971288696989989E-4</v>
       </c>
-      <c r="AJ42" s="5">
+      <c r="AJ42" s="4">
         <f t="shared" si="2"/>
         <v>9.3838240000000007E-3</v>
       </c>
-      <c r="AK42" s="5">
+      <c r="AK42" s="4">
         <f t="shared" si="2"/>
         <v>1.2197248999999999E-2</v>
       </c>
-      <c r="AL42" s="5"/>
-      <c r="AM42" s="5">
+      <c r="AL42" s="4"/>
+      <c r="AM42" s="4">
         <f t="shared" si="2"/>
         <v>2.681028499E-3</v>
       </c>
-      <c r="AN42" s="5">
+      <c r="AN42" s="4">
         <f t="shared" si="2"/>
         <v>9.8355990000000004E-3</v>
       </c>
-      <c r="AO42" s="5">
+      <c r="AO42" s="4">
         <f t="shared" si="2"/>
         <v>1.47346E-2</v>
       </c>
-      <c r="AP42" s="5"/>
-      <c r="AQ42" s="5">
+      <c r="AP42" s="4"/>
+      <c r="AQ42" s="4">
         <f t="shared" si="2"/>
         <v>2.4393440187000003E-3</v>
       </c>
-      <c r="AR42" s="5">
+      <c r="AR42" s="4">
         <f t="shared" si="2"/>
         <v>1.4072319E-2</v>
       </c>
-      <c r="AS42" s="5">
+      <c r="AS42" s="4">
         <f t="shared" si="2"/>
         <v>1.3270272E-2</v>
       </c>
@@ -2897,7 +4179,7 @@
         <v>8.9130910289983052E-3</v>
       </c>
       <c r="AA43">
-        <f t="shared" ref="Z43:AS43" si="5">_xlfn.STDEV.S(AA16:AA25)</f>
+        <f t="shared" ref="AA43:AS43" si="5">_xlfn.STDEV.S(AA16:AA25)</f>
         <v>2.7568081091165052E-3</v>
       </c>
       <c r="AB43">
@@ -3051,7 +4333,7 @@
         <v>1.2390371999999998</v>
       </c>
       <c r="X47" s="1">
-        <f t="shared" ref="X47:Z47" si="12">X16*180</f>
+        <f t="shared" ref="X47:Y47" si="12">X16*180</f>
         <v>1.1178306</v>
       </c>
       <c r="Y47" s="1">
@@ -3198,7 +4480,7 @@
         <v>1.0438829999999999</v>
       </c>
       <c r="X48" s="1">
-        <f t="shared" ref="X48:Z48" si="20">X17*180</f>
+        <f t="shared" ref="X48:Y48" si="20">X17*180</f>
         <v>0.72154080000000009</v>
       </c>
       <c r="Y48" s="1">
@@ -3345,7 +4627,7 @@
         <v>2.1832200000000002E-9</v>
       </c>
       <c r="X49" s="1">
-        <f t="shared" ref="X49:Z49" si="27">X18*180</f>
+        <f t="shared" ref="X49:Y49" si="27">X18*180</f>
         <v>1.9639979999999999</v>
       </c>
       <c r="Y49" s="1">
@@ -3492,7 +4774,7 @@
         <v>0.17020259999999998</v>
       </c>
       <c r="X50" s="1">
-        <f t="shared" ref="X50:Z50" si="34">X19*180</f>
+        <f t="shared" ref="X50:Y50" si="34">X19*180</f>
         <v>1.258542</v>
       </c>
       <c r="Y50" s="1">
@@ -3639,7 +4921,7 @@
         <v>0.24118560000000003</v>
       </c>
       <c r="X51" s="1">
-        <f t="shared" ref="X51:Z51" si="41">X20*180</f>
+        <f t="shared" ref="X51:Y51" si="41">X20*180</f>
         <v>0.89552700000000007</v>
       </c>
       <c r="Y51" s="1">
@@ -3786,7 +5068,7 @@
         <v>7.2941219999999995E-8</v>
       </c>
       <c r="X52" s="1">
-        <f t="shared" ref="X52:Z52" si="48">X21*180</f>
+        <f t="shared" ref="X52:Y52" si="48">X21*180</f>
         <v>2.3459219999999998</v>
       </c>
       <c r="Y52" s="1">
@@ -3933,7 +5215,7 @@
         <v>1.323234</v>
       </c>
       <c r="X53" s="1">
-        <f t="shared" ref="X53:Z53" si="55">X22*180</f>
+        <f t="shared" ref="X53:Y53" si="55">X22*180</f>
         <v>2.2754159999999999</v>
       </c>
       <c r="Y53" s="1">
@@ -4080,7 +5362,7 @@
         <v>0.48896459999999997</v>
       </c>
       <c r="X54" s="1">
-        <f t="shared" ref="X54:Z54" si="62">X23*180</f>
+        <f t="shared" ref="X54:Y54" si="62">X23*180</f>
         <v>1.2318245999999999</v>
       </c>
       <c r="Y54" s="1">
@@ -4227,7 +5509,7 @@
         <v>3.0419099999999998E-2</v>
       </c>
       <c r="X55" s="1">
-        <f t="shared" ref="X55:Z55" si="69">X24*180</f>
+        <f t="shared" ref="X55:Y55" si="69">X24*180</f>
         <v>0.84456719999999996</v>
       </c>
       <c r="Y55" s="1">
@@ -4374,7 +5656,7 @@
         <v>1.039158</v>
       </c>
       <c r="X56" s="1">
-        <f t="shared" ref="X56:Z56" si="76">X25*180</f>
+        <f t="shared" ref="X56:Y56" si="76">X25*180</f>
         <v>1.5802254</v>
       </c>
       <c r="Y56" s="1">
@@ -4526,145 +5808,145 @@
       <c r="A73" t="s">
         <v>13</v>
       </c>
-      <c r="C73" s="4">
+      <c r="C73" s="5">
         <f>AVERAGE(C47:C56)</f>
         <v>0.24754239180000001</v>
       </c>
-      <c r="D73" s="4">
+      <c r="D73" s="5">
         <f t="shared" ref="D73:E73" si="78">AVERAGE(D47:D56)</f>
         <v>1.2322834199999999</v>
       </c>
-      <c r="E73" s="4">
+      <c r="E73" s="5">
         <f t="shared" si="78"/>
         <v>1.30328226</v>
       </c>
-      <c r="F73" s="4"/>
-      <c r="G73" s="4">
+      <c r="F73" s="5"/>
+      <c r="G73" s="5">
         <f t="shared" ref="G73:I73" si="79">AVERAGE(G47:G56)</f>
         <v>0.46965892119839997</v>
       </c>
-      <c r="H73" s="4">
+      <c r="H73" s="5">
         <f t="shared" si="79"/>
         <v>1.18919826</v>
       </c>
-      <c r="I73" s="4">
+      <c r="I73" s="5">
         <f t="shared" si="79"/>
         <v>1.5640482599999999</v>
       </c>
-      <c r="J73" s="4"/>
-      <c r="K73" s="4">
+      <c r="J73" s="5"/>
+      <c r="K73" s="5">
         <f t="shared" ref="K73:S73" si="80">AVERAGE(K47:K56)</f>
         <v>0.18417429250477019</v>
       </c>
-      <c r="L73" s="4">
+      <c r="L73" s="5">
         <f t="shared" si="80"/>
         <v>1.1643208199999999</v>
       </c>
-      <c r="M73" s="4">
+      <c r="M73" s="5">
         <f t="shared" si="80"/>
         <v>1.30363308</v>
       </c>
-      <c r="N73" s="4"/>
-      <c r="O73" s="4">
+      <c r="N73" s="5"/>
+      <c r="O73" s="5">
         <f t="shared" si="80"/>
         <v>0.20378195676521926</v>
       </c>
-      <c r="P73" s="4">
+      <c r="P73" s="5">
         <f t="shared" si="80"/>
         <v>1.2302083799999999</v>
       </c>
-      <c r="Q73" s="4">
+      <c r="Q73" s="5">
         <f t="shared" si="80"/>
         <v>1.4668761600000002</v>
       </c>
-      <c r="R73" s="4"/>
-      <c r="S73" s="4">
+      <c r="R73" s="5"/>
+      <c r="S73" s="5">
         <f t="shared" si="80"/>
         <v>0.59497052973839992</v>
       </c>
-      <c r="T73" s="4">
+      <c r="T73" s="5">
         <f t="shared" ref="T73:U73" si="81">AVERAGE(T47:T56)</f>
         <v>2.3177989800000001</v>
       </c>
-      <c r="U73" s="4">
+      <c r="U73" s="5">
         <f t="shared" si="81"/>
         <v>2.5174241999999998</v>
       </c>
-      <c r="V73" s="4"/>
-      <c r="W73" s="4">
+      <c r="V73" s="5"/>
+      <c r="W73" s="5">
         <f t="shared" ref="W73:Y73" si="82">AVERAGE(W47:W56)</f>
         <v>0.55760841751244394</v>
       </c>
-      <c r="X73" s="4">
+      <c r="X73" s="5">
         <f t="shared" si="82"/>
         <v>1.4235393599999999</v>
       </c>
-      <c r="Y73" s="4">
+      <c r="Y73" s="5">
         <f t="shared" si="82"/>
         <v>2.2340986199999997</v>
       </c>
-      <c r="Z73" s="4"/>
-      <c r="AA73" s="4">
-        <f t="shared" ref="Z73:AS73" si="83">AVERAGE(AA47:AA56)</f>
+      <c r="Z73" s="5"/>
+      <c r="AA73" s="5">
+        <f t="shared" ref="AA73:AS73" si="83">AVERAGE(AA47:AA56)</f>
         <v>0.28466215965904068</v>
       </c>
-      <c r="AB73" s="4">
+      <c r="AB73" s="5">
         <f t="shared" si="83"/>
         <v>1.56164364</v>
       </c>
-      <c r="AC73" s="4">
+      <c r="AC73" s="5">
         <f t="shared" si="83"/>
         <v>2.3575332600000003</v>
       </c>
-      <c r="AD73" s="4"/>
-      <c r="AE73" s="4">
+      <c r="AD73" s="5"/>
+      <c r="AE73" s="5">
         <f t="shared" si="83"/>
         <v>0.41583975480000007</v>
       </c>
-      <c r="AF73" s="4">
+      <c r="AF73" s="5">
         <f t="shared" si="83"/>
         <v>1.5992967600000001</v>
       </c>
-      <c r="AG73" s="4">
+      <c r="AG73" s="5">
         <f t="shared" si="83"/>
         <v>1.8482945400000002</v>
       </c>
-      <c r="AH73" s="4"/>
-      <c r="AI73" s="4">
+      <c r="AH73" s="5"/>
+      <c r="AI73" s="5">
         <f t="shared" si="83"/>
         <v>0.17094831965458201</v>
       </c>
-      <c r="AJ73" s="4">
+      <c r="AJ73" s="5">
         <f t="shared" si="83"/>
         <v>1.6890883200000002</v>
       </c>
-      <c r="AK73" s="4">
+      <c r="AK73" s="5">
         <f t="shared" si="83"/>
         <v>2.19550482</v>
       </c>
-      <c r="AL73" s="4"/>
-      <c r="AM73" s="4">
+      <c r="AL73" s="5"/>
+      <c r="AM73" s="5">
         <f t="shared" si="83"/>
         <v>0.4825851298199999</v>
       </c>
-      <c r="AN73" s="4">
+      <c r="AN73" s="5">
         <f t="shared" si="83"/>
         <v>1.7704078200000002</v>
       </c>
-      <c r="AO73" s="4">
+      <c r="AO73" s="5">
         <f t="shared" si="83"/>
         <v>2.652228</v>
       </c>
-      <c r="AP73" s="4"/>
-      <c r="AQ73" s="4">
+      <c r="AP73" s="5"/>
+      <c r="AQ73" s="5">
         <f t="shared" si="83"/>
         <v>0.43908192336600005</v>
       </c>
-      <c r="AR73" s="4">
+      <c r="AR73" s="5">
         <f t="shared" si="83"/>
         <v>2.5330174200000002</v>
       </c>
-      <c r="AS73" s="4">
+      <c r="AS73" s="5">
         <f t="shared" si="83"/>
         <v>2.3886489599999998</v>
       </c>
@@ -4746,7 +6028,7 @@
         <v>1.6043563852196951</v>
       </c>
       <c r="AA74">
-        <f t="shared" ref="Z74:AS74" si="89">_xlfn.STDEV.S(AA47:AA56)</f>
+        <f t="shared" ref="AA74:AS74" si="89">_xlfn.STDEV.S(AA47:AA56)</f>
         <v>0.49622545964097092</v>
       </c>
       <c r="AB74">

</xml_diff>